<commit_message>
criando resumos procv + corresp
</commit_message>
<xml_diff>
--- a/2.Excel/hands-on/6.Funcoes_Mercado/10.CORRESP/1.CORRESP.xlsx
+++ b/2.Excel/hands-on/6.Funcoes_Mercado/10.CORRESP/1.CORRESP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projetos para Github\Hashtag\2.Excel\hands-on\6.Funcoes_Mercado\10.CORRESP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA445CE-35F9-43A1-85C7-AB29CE53E411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2998DD7B-85D7-408D-9039-9E50BC241B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12240" yWindow="120" windowWidth="10800" windowHeight="12792" activeTab="1" xr2:uid="{90D394A7-0334-4363-9DA1-420D95C76B52}"/>
+    <workbookView xWindow="12240" yWindow="120" windowWidth="10800" windowHeight="12792" firstSheet="2" activeTab="2" xr2:uid="{90D394A7-0334-4363-9DA1-420D95C76B52}"/>
   </bookViews>
   <sheets>
     <sheet name="CORRESP" sheetId="2" r:id="rId1"/>
@@ -2062,7 +2062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E71EB1-CED9-4CD0-84CB-E786CB6D5CED}">
   <dimension ref="A1:J309"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -3477,7 +3477,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C02D153-4518-406C-B717-C8680DD429E8}">
   <dimension ref="B2:H17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3788,60 +3790,60 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="14">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="C16" s="6">
         <f>VLOOKUP($B16,$B$3:$H$13,MATCH(C$15,$B$2:$H$2,0),0)</f>
-        <v>136909</v>
+        <v>230870</v>
       </c>
       <c r="D16" s="6">
         <f t="shared" ref="D16:H17" si="0">VLOOKUP($B16,$B$3:$H$13,MATCH(D$15,$B$2:$H$2,0),0)</f>
-        <v>827119</v>
+        <v>578927</v>
       </c>
       <c r="E16" s="6">
         <f t="shared" si="0"/>
-        <v>804873</v>
+        <v>56435</v>
       </c>
       <c r="F16" s="6">
         <f t="shared" si="0"/>
-        <v>701521</v>
+        <v>486895</v>
       </c>
       <c r="G16" s="6">
         <f t="shared" si="0"/>
-        <v>533749</v>
+        <v>251105</v>
       </c>
       <c r="H16" s="6">
         <f t="shared" si="0"/>
-        <v>570184</v>
+        <v>903436</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="14">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="C17" s="6">
         <f>VLOOKUP($B17,$B$3:$H$13,MATCH(C$15,$B$2:$H$2,0),0)</f>
-        <v>339849</v>
+        <v>136909</v>
       </c>
       <c r="D17" s="6">
         <f t="shared" si="0"/>
-        <v>142492</v>
+        <v>827119</v>
       </c>
       <c r="E17" s="6">
         <f t="shared" si="0"/>
-        <v>488286</v>
+        <v>804873</v>
       </c>
       <c r="F17" s="6">
         <f t="shared" si="0"/>
-        <v>520411</v>
+        <v>701521</v>
       </c>
       <c r="G17" s="6">
         <f t="shared" si="0"/>
-        <v>349757</v>
+        <v>533749</v>
       </c>
       <c r="H17" s="6">
         <f t="shared" si="0"/>
-        <v>726040</v>
+        <v>570184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>